<commit_message>
Add current_date as input parameter in the file
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmisra/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmisra/GitHub/chime/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C801501-657E-D74C-8964-65CA6A486E39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A250E-C946-E644-8B83-46703C887DC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{629496A2-78F5-45B0-9460-8F7D70EBC313}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Severe</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>DATE_FIRST_HOSPITALIZED</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133B2CA5-8539-104E-B0AE-797D51410EEB}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -469,10 +472,10 @@
     <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -521,8 +524,11 @@
       <c r="P1" t="s">
         <v>18</v>
       </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -571,8 +577,12 @@
       <c r="P2" s="5">
         <v>43911</v>
       </c>
+      <c r="Q2" s="5">
+        <f ca="1">TODAY()</f>
+        <v>43942</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -620,11 +630,15 @@
       </c>
       <c r="P3" s="5">
         <v>43911</v>
+      </c>
+      <c r="Q3" s="5">
+        <f ca="1">TODAY()</f>
+        <v>43942</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date" error="Valid date format e.g. 3/21/20" sqref="P2:P3" xr:uid="{DC6A8CA9-9F02-104D-A28F-30AC021BAAEE}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date" error="Valid date format e.g. 3/21/20" sqref="P2:Q3" xr:uid="{DC6A8CA9-9F02-104D-A28F-30AC021BAAEE}">
       <formula1>43466</formula1>
       <formula2>44197</formula2>
     </dataValidation>

</xml_diff>